<commit_message>
weather monitoring stations & matching
</commit_message>
<xml_diff>
--- a/pm10/_02processing/_02output/_00-3matching/matching_sigungu.xlsx
+++ b/pm10/_02processing/_02output/_00-3matching/matching_sigungu.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="375" windowWidth="28035" windowHeight="12765" firstSheet="2" activeTab="10"/>
+    <workbookView xWindow="360" yWindow="375" windowWidth="28035" windowHeight="12765" firstSheet="7" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="행정구역" sheetId="3" r:id="rId1"/>
@@ -3677,10 +3677,10 @@
     <t>SIG_CD</t>
   </si>
   <si>
-    <t>join_CODE</t>
-  </si>
-  <si>
     <t>거리기반</t>
+  </si>
+  <si>
+    <t>join_code</t>
   </si>
 </sst>
 </file>
@@ -13362,14 +13362,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B251"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
+      <selection activeCell="D230" sqref="D230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.75" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.625" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="9.625" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -13377,7 +13377,7 @@
         <v>1174</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -13665,7 +13665,7 @@
         <v>874</v>
       </c>
       <c r="B37" s="13">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -13809,7 +13809,7 @@
         <v>892</v>
       </c>
       <c r="B55" s="13">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
@@ -13841,7 +13841,7 @@
         <v>896</v>
       </c>
       <c r="B59" s="13">
-        <v>256</v>
+        <v>156</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
@@ -13881,7 +13881,7 @@
         <v>901</v>
       </c>
       <c r="B64" s="13">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
@@ -13929,7 +13929,7 @@
         <v>907</v>
       </c>
       <c r="B70" s="13">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
@@ -14009,7 +14009,7 @@
         <v>917</v>
       </c>
       <c r="B80" s="13">
-        <v>102</v>
+        <v>201</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
@@ -14057,7 +14057,7 @@
         <v>923</v>
       </c>
       <c r="B86" s="13">
-        <v>232</v>
+        <v>131</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
@@ -14193,7 +14193,7 @@
         <v>940</v>
       </c>
       <c r="B103" s="13">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
@@ -14201,7 +14201,7 @@
         <v>941</v>
       </c>
       <c r="B104" s="13">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
@@ -14217,7 +14217,7 @@
         <v>943</v>
       </c>
       <c r="B106" s="13">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
@@ -14225,7 +14225,7 @@
         <v>944</v>
       </c>
       <c r="B107" s="13">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
@@ -14233,7 +14233,7 @@
         <v>945</v>
       </c>
       <c r="B108" s="13">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
@@ -14305,7 +14305,7 @@
         <v>954</v>
       </c>
       <c r="B117" s="13">
-        <v>257</v>
+        <v>159</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
@@ -14433,7 +14433,7 @@
         <v>970</v>
       </c>
       <c r="B133" s="13">
-        <v>176</v>
+        <v>143</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
@@ -14441,7 +14441,7 @@
         <v>971</v>
       </c>
       <c r="B134" s="13">
-        <v>176</v>
+        <v>143</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
@@ -14449,7 +14449,7 @@
         <v>972</v>
       </c>
       <c r="B135" s="13">
-        <v>176</v>
+        <v>143</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
@@ -14465,7 +14465,7 @@
         <v>974</v>
       </c>
       <c r="B137" s="13">
-        <v>176</v>
+        <v>143</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
@@ -14649,7 +14649,7 @@
         <v>997</v>
       </c>
       <c r="B160" s="13">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
@@ -14697,7 +14697,7 @@
         <v>1003</v>
       </c>
       <c r="B166" s="13">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.3">
@@ -14761,7 +14761,7 @@
         <v>1011</v>
       </c>
       <c r="B174" s="13">
-        <v>155</v>
+        <v>255</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.3">
@@ -14937,7 +14937,7 @@
         <v>1033</v>
       </c>
       <c r="B196" s="13">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.3">
@@ -14945,7 +14945,7 @@
         <v>1034</v>
       </c>
       <c r="B197" s="13">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.3">
@@ -14953,7 +14953,7 @@
         <v>1035</v>
       </c>
       <c r="B198" s="13">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.3">
@@ -14969,7 +14969,7 @@
         <v>1037</v>
       </c>
       <c r="B200" s="13">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
@@ -14977,7 +14977,7 @@
         <v>1038</v>
       </c>
       <c r="B201" s="13">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.3">
@@ -14993,7 +14993,7 @@
         <v>1040</v>
       </c>
       <c r="B203" s="13">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.3">
@@ -15025,7 +15025,7 @@
         <v>1044</v>
       </c>
       <c r="B207" s="13">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.3">
@@ -15057,7 +15057,7 @@
         <v>1048</v>
       </c>
       <c r="B211" s="13">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.3">
@@ -15089,7 +15089,7 @@
         <v>1052</v>
       </c>
       <c r="B215" s="13">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.3">
@@ -15113,7 +15113,7 @@
         <v>1055</v>
       </c>
       <c r="B218" s="13">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.3">
@@ -15201,7 +15201,7 @@
         <v>1066</v>
       </c>
       <c r="B229" s="13">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.3">
@@ -15225,7 +15225,7 @@
         <v>1069</v>
       </c>
       <c r="B232" s="13">
-        <v>202</v>
+        <v>101</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.3">
@@ -15289,7 +15289,7 @@
         <v>1077</v>
       </c>
       <c r="B240" s="13">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.3">
@@ -15321,7 +15321,7 @@
         <v>1081</v>
       </c>
       <c r="B244" s="13">
-        <v>100</v>
+        <v>217</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.3">
@@ -15401,7 +15401,7 @@
         <v>1139</v>
       </c>
       <c r="C1" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -57218,7 +57218,7 @@
         <v>1173</v>
       </c>
       <c r="H1" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="K1" t="s">
         <v>819</v>
@@ -57385,7 +57385,7 @@
       </c>
       <c r="G6">
         <f>VLOOKUP(A6,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H6">
         <v>108</v>
@@ -57453,7 +57453,7 @@
       </c>
       <c r="G8">
         <f>VLOOKUP(A8,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H8">
         <v>108</v>
@@ -57487,7 +57487,7 @@
       </c>
       <c r="G9">
         <f>VLOOKUP(A9,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H9">
         <v>108</v>
@@ -57623,7 +57623,7 @@
       </c>
       <c r="G13">
         <f>VLOOKUP(A13,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H13">
         <v>108</v>
@@ -57725,7 +57725,7 @@
       </c>
       <c r="G16">
         <f>VLOOKUP(A16,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H16">
         <v>108</v>
@@ -58209,7 +58209,7 @@
       </c>
       <c r="G30">
         <f>VLOOKUP(A30,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>102</v>
+        <v>201</v>
       </c>
       <c r="H30">
         <v>102</v>
@@ -58455,7 +58455,7 @@
       </c>
       <c r="G37">
         <f>VLOOKUP(A37,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>202</v>
+        <v>101</v>
       </c>
       <c r="H37">
         <v>202</v>
@@ -58567,7 +58567,7 @@
       </c>
       <c r="G40">
         <f>VLOOKUP(A40,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="H40">
         <v>119</v>
@@ -58673,7 +58673,7 @@
       </c>
       <c r="G43">
         <f>VLOOKUP(A43,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H43">
         <v>108</v>
@@ -58707,7 +58707,7 @@
       </c>
       <c r="G44">
         <f>VLOOKUP(A44,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="H44">
         <v>95</v>
@@ -59029,7 +59029,7 @@
       </c>
       <c r="G53">
         <f>VLOOKUP(A53,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H53">
         <v>108</v>
@@ -59097,7 +59097,7 @@
       </c>
       <c r="G55">
         <f>VLOOKUP(A55,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="H55">
         <v>108</v>
@@ -59277,7 +59277,7 @@
       </c>
       <c r="G60">
         <f>VLOOKUP(A60,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="H60">
         <v>108</v>
@@ -59348,7 +59348,7 @@
       </c>
       <c r="G62">
         <f>VLOOKUP(A62,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H62">
         <v>108</v>
@@ -59420,7 +59420,7 @@
       </c>
       <c r="G64">
         <f>VLOOKUP(A64,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H64">
         <v>108</v>
@@ -59457,7 +59457,7 @@
       </c>
       <c r="G65">
         <f>VLOOKUP(A65,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="H65">
         <v>108</v>
@@ -59602,7 +59602,7 @@
       </c>
       <c r="G69">
         <f>VLOOKUP(A69,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H69">
         <v>108</v>
@@ -59676,7 +59676,7 @@
       </c>
       <c r="G71">
         <f>VLOOKUP(A71,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="H71">
         <v>108</v>
@@ -59959,7 +59959,7 @@
       </c>
       <c r="G79">
         <f>VLOOKUP(A79,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="H79">
         <v>214</v>
@@ -61454,7 +61454,7 @@
       </c>
       <c r="G120">
         <f>VLOOKUP(A120,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>176</v>
+        <v>143</v>
       </c>
       <c r="H120">
         <v>176</v>
@@ -61560,7 +61560,7 @@
       </c>
       <c r="G123">
         <f>VLOOKUP(A123,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>176</v>
+        <v>143</v>
       </c>
       <c r="H123">
         <v>176</v>
@@ -61594,7 +61594,7 @@
       </c>
       <c r="G124">
         <f>VLOOKUP(A124,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>176</v>
+        <v>143</v>
       </c>
       <c r="H124">
         <v>176</v>
@@ -61628,7 +61628,7 @@
       </c>
       <c r="G125">
         <f>VLOOKUP(A125,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>176</v>
+        <v>143</v>
       </c>
       <c r="H125">
         <v>176</v>
@@ -61806,7 +61806,7 @@
       </c>
       <c r="G130">
         <f>VLOOKUP(A130,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="H130">
         <v>146</v>
@@ -62148,7 +62148,7 @@
       </c>
       <c r="G139">
         <f>VLOOKUP(A139,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>155</v>
+        <v>255</v>
       </c>
       <c r="H139">
         <v>155</v>
@@ -62930,7 +62930,7 @@
       </c>
       <c r="G161">
         <f>VLOOKUP(A161,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>257</v>
+        <v>159</v>
       </c>
       <c r="H161">
         <v>257</v>
@@ -63558,7 +63558,7 @@
       </c>
       <c r="G179">
         <f>VLOOKUP(A179,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>256</v>
+        <v>156</v>
       </c>
       <c r="H179">
         <v>256</v>

</xml_diff>

<commit_message>
after weather monitoring station preprocessing
</commit_message>
<xml_diff>
--- a/pm10/_02processing/_02output/_00-3matching/matching_sigungu.xlsx
+++ b/pm10/_02processing/_02output/_00-3matching/matching_sigungu.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="375" windowWidth="28035" windowHeight="12765" firstSheet="7" activeTab="10"/>
+    <workbookView xWindow="360" yWindow="435" windowWidth="28035" windowHeight="12705" firstSheet="2" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="행정구역" sheetId="3" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Sheet1" sheetId="9" r:id="rId10"/>
     <sheet name="spatialJoin" sheetId="11" r:id="rId11"/>
     <sheet name="Sheet2" sheetId="12" r:id="rId12"/>
+    <sheet name="대상시군구2" sheetId="13" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">기상기후!$A$1:$Q$230</definedName>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9339" uniqueCount="1177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9340" uniqueCount="1178">
   <si>
     <t>서울</t>
   </si>
@@ -3681,6 +3682,9 @@
   </si>
   <si>
     <t>join_code</t>
+  </si>
+  <si>
+    <t>sig_cd</t>
   </si>
 </sst>
 </file>
@@ -13362,14 +13366,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
-      <selection activeCell="D230" sqref="D230"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="9.625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.625" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -13737,7 +13741,7 @@
         <v>883</v>
       </c>
       <c r="B46" s="13">
-        <v>254</v>
+        <v>244</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -13745,7 +13749,7 @@
         <v>884</v>
       </c>
       <c r="B47" s="13">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -13777,7 +13781,7 @@
         <v>888</v>
       </c>
       <c r="B51" s="13">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -13793,7 +13797,7 @@
         <v>890</v>
       </c>
       <c r="B53" s="13">
-        <v>266</v>
+        <v>168</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
@@ -13801,7 +13805,7 @@
         <v>891</v>
       </c>
       <c r="B54" s="13">
-        <v>254</v>
+        <v>156</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
@@ -13809,7 +13813,7 @@
         <v>892</v>
       </c>
       <c r="B55" s="13">
-        <v>254</v>
+        <v>247</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
@@ -13833,7 +13837,7 @@
         <v>895</v>
       </c>
       <c r="B58" s="13">
-        <v>258</v>
+        <v>262</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -13857,7 +13861,7 @@
         <v>898</v>
       </c>
       <c r="B61" s="13">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
@@ -13889,7 +13893,7 @@
         <v>902</v>
       </c>
       <c r="B65" s="13">
-        <v>252</v>
+        <v>156</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
@@ -13897,7 +13901,7 @@
         <v>903</v>
       </c>
       <c r="B66" s="13">
-        <v>252</v>
+        <v>156</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
@@ -13905,7 +13909,7 @@
         <v>904</v>
       </c>
       <c r="B67" s="13">
-        <v>251</v>
+        <v>156</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
@@ -13921,7 +13925,7 @@
         <v>906</v>
       </c>
       <c r="B69" s="13">
-        <v>268</v>
+        <v>261</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
@@ -14321,7 +14325,7 @@
         <v>956</v>
       </c>
       <c r="B119" s="13">
-        <v>257</v>
+        <v>159</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
@@ -14345,7 +14349,7 @@
         <v>959</v>
       </c>
       <c r="B122" s="13">
-        <v>257</v>
+        <v>159</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
@@ -14353,7 +14357,7 @@
         <v>960</v>
       </c>
       <c r="B123" s="13">
-        <v>253</v>
+        <v>159</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
@@ -14385,7 +14389,7 @@
         <v>964</v>
       </c>
       <c r="B127" s="13">
-        <v>257</v>
+        <v>159</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
@@ -14553,7 +14557,7 @@
         <v>985</v>
       </c>
       <c r="B148" s="13">
-        <v>283</v>
+        <v>138</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
@@ -14601,7 +14605,7 @@
         <v>991</v>
       </c>
       <c r="B154" s="13">
-        <v>137</v>
+        <v>273</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
@@ -14641,7 +14645,7 @@
         <v>996</v>
       </c>
       <c r="B159" s="13">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
@@ -14729,7 +14733,7 @@
         <v>1007</v>
       </c>
       <c r="B170" s="13">
-        <v>255</v>
+        <v>155</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.3">
@@ -14737,7 +14741,7 @@
         <v>1008</v>
       </c>
       <c r="B171" s="13">
-        <v>255</v>
+        <v>155</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.3">
@@ -14761,7 +14765,7 @@
         <v>1011</v>
       </c>
       <c r="B174" s="13">
-        <v>255</v>
+        <v>155</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.3">
@@ -14793,7 +14797,7 @@
         <v>1015</v>
       </c>
       <c r="B178" s="13">
-        <v>253</v>
+        <v>159</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.3">
@@ -14817,7 +14821,7 @@
         <v>1018</v>
       </c>
       <c r="B181" s="13">
-        <v>257</v>
+        <v>288</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.3">
@@ -14825,7 +14829,7 @@
         <v>1019</v>
       </c>
       <c r="B182" s="13">
-        <v>263</v>
+        <v>285</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.3">
@@ -14833,7 +14837,7 @@
         <v>1020</v>
       </c>
       <c r="B183" s="13">
-        <v>263</v>
+        <v>155</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.3">
@@ -14865,7 +14869,7 @@
         <v>1024</v>
       </c>
       <c r="B187" s="13">
-        <v>266</v>
+        <v>192</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.3">
@@ -14881,7 +14885,7 @@
         <v>1026</v>
       </c>
       <c r="B189" s="13">
-        <v>264</v>
+        <v>289</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.3">
@@ -15049,7 +15053,7 @@
         <v>1047</v>
       </c>
       <c r="B210" s="13">
-        <v>99</v>
+        <v>108</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.3">
@@ -15145,7 +15149,7 @@
         <v>1059</v>
       </c>
       <c r="B222" s="13">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.3">
@@ -15321,7 +15325,7 @@
         <v>1081</v>
       </c>
       <c r="B244" s="13">
-        <v>217</v>
+        <v>100</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.3">
@@ -15329,7 +15333,7 @@
         <v>1082</v>
       </c>
       <c r="B245" s="13">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.3">
@@ -15345,7 +15349,7 @@
         <v>1084</v>
       </c>
       <c r="B247" s="13">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.3">
@@ -15391,7 +15395,7 @@
   <dimension ref="A1:C182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -15720,7 +15724,7 @@
         <v>917</v>
       </c>
       <c r="C30">
-        <v>102</v>
+        <v>201</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -15797,7 +15801,7 @@
         <v>1069</v>
       </c>
       <c r="C37">
-        <v>202</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -15830,7 +15834,7 @@
         <v>1044</v>
       </c>
       <c r="C40">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -15874,7 +15878,7 @@
         <v>1066</v>
       </c>
       <c r="C44">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -15918,7 +15922,7 @@
         <v>1059</v>
       </c>
       <c r="C48">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -15995,7 +15999,7 @@
         <v>1052</v>
       </c>
       <c r="C55">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
@@ -16050,7 +16054,7 @@
         <v>1038</v>
       </c>
       <c r="C60">
-        <v>108</v>
+        <v>119</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
@@ -16105,7 +16109,7 @@
         <v>1035</v>
       </c>
       <c r="C65">
-        <v>108</v>
+        <v>119</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
@@ -16171,7 +16175,7 @@
         <v>1037</v>
       </c>
       <c r="C71">
-        <v>108</v>
+        <v>119</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
@@ -16259,7 +16263,7 @@
         <v>1077</v>
       </c>
       <c r="C79">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
@@ -16292,7 +16296,7 @@
         <v>1082</v>
       </c>
       <c r="C82">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
@@ -16611,7 +16615,7 @@
         <v>985</v>
       </c>
       <c r="C111">
-        <v>283</v>
+        <v>138</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
@@ -16710,7 +16714,7 @@
         <v>974</v>
       </c>
       <c r="C120">
-        <v>176</v>
+        <v>143</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
@@ -16743,7 +16747,7 @@
         <v>971</v>
       </c>
       <c r="C123">
-        <v>176</v>
+        <v>143</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
@@ -16754,7 +16758,7 @@
         <v>970</v>
       </c>
       <c r="C124">
-        <v>176</v>
+        <v>143</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
@@ -16765,7 +16769,7 @@
         <v>972</v>
       </c>
       <c r="C125">
-        <v>176</v>
+        <v>143</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
@@ -16809,7 +16813,7 @@
         <v>884</v>
       </c>
       <c r="C129">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
@@ -16820,7 +16824,7 @@
         <v>874</v>
       </c>
       <c r="C130">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
@@ -16908,7 +16912,7 @@
         <v>1008</v>
       </c>
       <c r="C138">
-        <v>255</v>
+        <v>155</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
@@ -16941,7 +16945,7 @@
         <v>1007</v>
       </c>
       <c r="C141">
-        <v>255</v>
+        <v>155</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
@@ -16963,7 +16967,7 @@
         <v>1015</v>
       </c>
       <c r="C143">
-        <v>253</v>
+        <v>159</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
@@ -16985,7 +16989,7 @@
         <v>1018</v>
       </c>
       <c r="C145">
-        <v>257</v>
+        <v>288</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
@@ -17018,7 +17022,7 @@
         <v>1024</v>
       </c>
       <c r="C148">
-        <v>266</v>
+        <v>192</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
@@ -17106,7 +17110,7 @@
         <v>964</v>
       </c>
       <c r="C156">
-        <v>257</v>
+        <v>159</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
@@ -17117,7 +17121,7 @@
         <v>960</v>
       </c>
       <c r="C157">
-        <v>253</v>
+        <v>159</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
@@ -17150,7 +17154,7 @@
         <v>956</v>
       </c>
       <c r="C160">
-        <v>257</v>
+        <v>159</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
@@ -17161,7 +17165,7 @@
         <v>954</v>
       </c>
       <c r="C161">
-        <v>257</v>
+        <v>159</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
@@ -17172,7 +17176,7 @@
         <v>959</v>
       </c>
       <c r="C162">
-        <v>257</v>
+        <v>159</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
@@ -17326,7 +17330,7 @@
         <v>890</v>
       </c>
       <c r="C176">
-        <v>266</v>
+        <v>168</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
@@ -17359,7 +17363,7 @@
         <v>896</v>
       </c>
       <c r="C179">
-        <v>256</v>
+        <v>156</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
@@ -17370,7 +17374,7 @@
         <v>888</v>
       </c>
       <c r="C180">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
@@ -17393,6 +17397,927 @@
       </c>
       <c r="C182">
         <v>189</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A181"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="P186" sqref="P186"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>42150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>42820</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>42800</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>42130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>41290</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>41210</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>41310</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>41410</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>41360</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>41190</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>41131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>41135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>41117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>41115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>41390</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>41273</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>41271</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>41173</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>41171</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>41461</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>41150</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>41220</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>48250</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>48170</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>48123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>48129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>48121</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>48127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>47130</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>47190</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>47150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>47170</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>47770</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>47940</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>47111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>29200</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>29110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>29170</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>29140</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>27200</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>27140</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>27230</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>27170</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>27260</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>27110</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>30230</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>30200</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>30140</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>26410</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>26290</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>26230</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>26320</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>26530</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>26380</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>26470</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>26200</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>26110</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>11680</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>11740</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>11305</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>11500</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>11620</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>11215</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>11530</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>11545</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>11350</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>11320</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>11230</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>11590</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>11440</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>11410</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>11650</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>11200</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>11290</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>11710</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>11470</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>11560</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>11170</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>11380</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>11110</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>11140</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>11260</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>31140</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>31170</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>31710</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>31110</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>28710</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>28170</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>28200</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>28140</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>28237</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>28260</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>28110</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>46230</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>46110</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>46150</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>46130</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>46830</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>45130</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>45140</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>45111</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>45113</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>50110</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>44210</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>44131</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>43150</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>43114</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>43113</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>42110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>41281</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>41570</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <v>41500</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <v>48310</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <v>48330</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <v>47210</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <v>45750</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <v>43760</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <v>41370</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <v>41430</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <v>41650</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <v>41450</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A124">
+        <v>26440</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A125">
+        <v>26710</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A126">
+        <v>26500</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <v>50130</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <v>43130</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A129">
+        <v>41285</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A130">
+        <v>27290</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A131">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A132">
+        <v>43111</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A133">
+        <v>42170</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A134">
+        <v>41111</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A135">
+        <v>48880</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A136">
+        <v>27710</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A137">
+        <v>26260</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A138">
+        <v>31200</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A139">
+        <v>44150</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A140">
+        <v>30110</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A141">
+        <v>42770</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A142">
+        <v>41480</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A143">
+        <v>41590</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A144">
+        <v>30170</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A145">
+        <v>44270</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A146">
+        <v>44133</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A147">
+        <v>47230</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A148">
+        <v>29155</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A149">
+        <v>28185</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A150">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A151">
+        <v>26350</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A152">
+        <v>41630</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A153">
+        <v>41250</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A154">
+        <v>41465</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A155">
+        <v>28245</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A156">
+        <v>42230</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A157">
+        <v>41113</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A158">
+        <v>42730</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A159">
+        <v>41610</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A160">
+        <v>41463</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A161">
+        <v>47730</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A162">
+        <v>28720</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A163">
+        <v>46790</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A164">
+        <v>44200</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A165">
+        <v>48850</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A166">
+        <v>41550</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A167">
+        <v>41133</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A168">
+        <v>45790</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A169">
+        <v>41830</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A170">
+        <v>41800</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A171">
+        <v>41820</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A172">
+        <v>26170</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A173">
+        <v>43800</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A174">
+        <v>47290</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A175">
+        <v>48240</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A176">
+        <v>26140</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A177">
+        <v>41670</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A178">
+        <v>47113</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A179">
+        <v>45800</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A180">
+        <v>45210</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A181">
+        <v>43750</v>
       </c>
     </row>
   </sheetData>
@@ -57187,8 +58112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M230"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -58212,7 +59137,7 @@
         <v>201</v>
       </c>
       <c r="H30">
-        <v>102</v>
+        <v>201</v>
       </c>
       <c r="K30">
         <v>28</v>
@@ -58458,7 +59383,7 @@
         <v>101</v>
       </c>
       <c r="H37">
-        <v>202</v>
+        <v>101</v>
       </c>
       <c r="K37">
         <v>35</v>
@@ -58570,7 +59495,7 @@
         <v>112</v>
       </c>
       <c r="H40">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="K40">
         <v>38</v>
@@ -58710,7 +59635,7 @@
         <v>98</v>
       </c>
       <c r="H44">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="K44">
         <v>42</v>
@@ -58850,10 +59775,10 @@
       </c>
       <c r="G48">
         <f>VLOOKUP(A48,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H48">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K48">
         <v>46</v>
@@ -59100,7 +60025,7 @@
         <v>112</v>
       </c>
       <c r="H55">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="K55">
         <v>53</v>
@@ -59280,7 +60205,7 @@
         <v>119</v>
       </c>
       <c r="H60">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="K60">
         <v>58</v>
@@ -59460,7 +60385,7 @@
         <v>119</v>
       </c>
       <c r="H65">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="K65">
         <v>63</v>
@@ -59679,7 +60604,7 @@
         <v>119</v>
       </c>
       <c r="H71">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="K71">
         <v>69</v>
@@ -59962,7 +60887,7 @@
         <v>216</v>
       </c>
       <c r="H79">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="K79">
         <v>77</v>
@@ -60069,10 +60994,10 @@
       </c>
       <c r="G82">
         <f>VLOOKUP(A82,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H82">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K82">
         <v>80</v>
@@ -61125,10 +62050,10 @@
       </c>
       <c r="G111">
         <f>VLOOKUP(A111,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>283</v>
+        <v>138</v>
       </c>
       <c r="H111">
-        <v>283</v>
+        <v>138</v>
       </c>
       <c r="K111">
         <v>109</v>
@@ -61457,7 +62382,7 @@
         <v>143</v>
       </c>
       <c r="H120">
-        <v>176</v>
+        <v>143</v>
       </c>
       <c r="K120">
         <v>118</v>
@@ -61563,7 +62488,7 @@
         <v>143</v>
       </c>
       <c r="H123">
-        <v>176</v>
+        <v>143</v>
       </c>
       <c r="K123">
         <v>121</v>
@@ -61597,7 +62522,7 @@
         <v>143</v>
       </c>
       <c r="H124">
-        <v>176</v>
+        <v>143</v>
       </c>
       <c r="K124">
         <v>122</v>
@@ -61631,7 +62556,7 @@
         <v>143</v>
       </c>
       <c r="H125">
-        <v>176</v>
+        <v>143</v>
       </c>
       <c r="K125">
         <v>123</v>
@@ -61772,10 +62697,10 @@
       </c>
       <c r="G129">
         <f>VLOOKUP(A129,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="H129">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="K129">
         <v>127</v>
@@ -61809,7 +62734,7 @@
         <v>140</v>
       </c>
       <c r="H130">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="K130">
         <v>128</v>
@@ -62111,10 +63036,10 @@
       </c>
       <c r="G138">
         <f>VLOOKUP(A138,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>255</v>
+        <v>155</v>
       </c>
       <c r="H138">
-        <v>255</v>
+        <v>155</v>
       </c>
       <c r="K138">
         <v>136</v>
@@ -62148,7 +63073,7 @@
       </c>
       <c r="G139">
         <f>VLOOKUP(A139,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>255</v>
+        <v>155</v>
       </c>
       <c r="H139">
         <v>155</v>
@@ -62223,10 +63148,10 @@
       </c>
       <c r="G141">
         <f>VLOOKUP(A141,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>255</v>
+        <v>155</v>
       </c>
       <c r="H141">
-        <v>255</v>
+        <v>155</v>
       </c>
       <c r="K141">
         <v>139</v>
@@ -62299,10 +63224,10 @@
       </c>
       <c r="G143">
         <f>VLOOKUP(A143,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>253</v>
+        <v>159</v>
       </c>
       <c r="H143">
-        <v>253</v>
+        <v>159</v>
       </c>
       <c r="K143">
         <v>141</v>
@@ -62374,10 +63299,10 @@
       </c>
       <c r="G145">
         <f>VLOOKUP(A145,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>257</v>
+        <v>288</v>
       </c>
       <c r="H145">
-        <v>257</v>
+        <v>288</v>
       </c>
       <c r="K145">
         <v>143</v>
@@ -62480,10 +63405,10 @@
       </c>
       <c r="G148">
         <f>VLOOKUP(A148,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>266</v>
+        <v>192</v>
       </c>
       <c r="H148">
-        <v>266</v>
+        <v>192</v>
       </c>
       <c r="K148">
         <v>146</v>
@@ -62760,10 +63685,10 @@
       </c>
       <c r="G156">
         <f>VLOOKUP(A156,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>257</v>
+        <v>159</v>
       </c>
       <c r="H156">
-        <v>257</v>
+        <v>159</v>
       </c>
       <c r="K156">
         <v>154</v>
@@ -62794,10 +63719,10 @@
       </c>
       <c r="G157">
         <f>VLOOKUP(A157,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>253</v>
+        <v>159</v>
       </c>
       <c r="H157">
-        <v>253</v>
+        <v>159</v>
       </c>
       <c r="K157">
         <v>155</v>
@@ -62896,10 +63821,10 @@
       </c>
       <c r="G160">
         <f>VLOOKUP(A160,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>257</v>
+        <v>159</v>
       </c>
       <c r="H160">
-        <v>257</v>
+        <v>159</v>
       </c>
       <c r="K160">
         <v>158</v>
@@ -62933,7 +63858,7 @@
         <v>159</v>
       </c>
       <c r="H161">
-        <v>257</v>
+        <v>159</v>
       </c>
       <c r="K161">
         <v>159</v>
@@ -62964,10 +63889,10 @@
       </c>
       <c r="G162">
         <f>VLOOKUP(A162,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>257</v>
+        <v>159</v>
       </c>
       <c r="H162">
-        <v>257</v>
+        <v>159</v>
       </c>
       <c r="K162">
         <v>160</v>
@@ -63452,10 +64377,10 @@
       </c>
       <c r="G176">
         <f>VLOOKUP(A176,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>266</v>
+        <v>168</v>
       </c>
       <c r="H176">
-        <v>266</v>
+        <v>168</v>
       </c>
       <c r="K176">
         <v>174</v>
@@ -63561,7 +64486,7 @@
         <v>156</v>
       </c>
       <c r="H179">
-        <v>256</v>
+        <v>156</v>
       </c>
       <c r="K179">
         <v>177</v>
@@ -63596,10 +64521,10 @@
       </c>
       <c r="G180">
         <f>VLOOKUP(A180,spatialJoin!$A$2:$B$251,2,FALSE)</f>
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="H180">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="K180">
         <v>178</v>

</xml_diff>